<commit_message>
add ESRM20 model results
</commit_message>
<xml_diff>
--- a/loss_data/selected_damaging_events/losses_selected_damaging_events.xlsx
+++ b/loss_data/selected_damaging_events/losses_selected_damaging_events.xlsx
@@ -5,15 +5,16 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_scenario_tests/loss_data/curated_events/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_scenario_tests/loss_data/selected_damaging_events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2511CFE5-3F0F-0A41-A8D3-F7E9419DA16D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD295FD-52FE-F547-A354-BF51953348C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2260" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Events!$A$2:$A$51</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="114">
   <si>
     <t>Source</t>
   </si>
@@ -331,6 +332,45 @@
   </si>
   <si>
     <t>CPI</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>eco_mean</t>
+  </si>
+  <si>
+    <t>eco_median</t>
+  </si>
+  <si>
+    <t>eco_5</t>
+  </si>
+  <si>
+    <t>eco_95</t>
+  </si>
+  <si>
+    <t>fatality_mean</t>
+  </si>
+  <si>
+    <t>fatality_median</t>
+  </si>
+  <si>
+    <t>fatality_5</t>
+  </si>
+  <si>
+    <t>fatality_95</t>
+  </si>
+  <si>
+    <t>Total Mean Damages ($M)</t>
+  </si>
+  <si>
+    <t>Total Mean Deaths</t>
+  </si>
+  <si>
+    <t>ESRM20 - Rupure Model</t>
+  </si>
+  <si>
+    <t>ESRM20 - ShakeMaps</t>
   </si>
 </sst>
 </file>
@@ -383,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,8 +442,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -489,6 +535,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -663,7 +718,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -707,6 +762,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,6 +953,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5CB4E6"/>
+      <color rgb="FF8BF1FF"/>
+      <color rgb="FF32617D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1219,13 +1294,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,9 +1319,13 @@
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="24.5" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17"/>
       <c r="B1" s="20" t="s">
         <v>90</v>
@@ -1265,8 +1344,16 @@
       <c r="N1" s="22"/>
       <c r="O1" s="19"/>
       <c r="P1" s="8"/>
-    </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" s="27"/>
+      <c r="S1" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="T1" s="27"/>
+    </row>
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -1315,8 +1402,20 @@
       <c r="P2" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q2" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
@@ -1355,8 +1454,20 @@
       <c r="P3" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q3" s="25">
+        <v>857</v>
+      </c>
+      <c r="R3" s="25">
+        <v>18760</v>
+      </c>
+      <c r="S3" s="25">
+        <v>682</v>
+      </c>
+      <c r="T3" s="25">
+        <v>23601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
@@ -1397,8 +1508,20 @@
       <c r="P4" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q4" s="25">
+        <v>195</v>
+      </c>
+      <c r="R4" s="25">
+        <v>1880</v>
+      </c>
+      <c r="S4" s="25">
+        <v>2041</v>
+      </c>
+      <c r="T4" s="25">
+        <v>37368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -1417,8 +1540,20 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="12"/>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q5" s="25">
+        <v>228</v>
+      </c>
+      <c r="R5" s="25">
+        <v>2552</v>
+      </c>
+      <c r="S5" s="25">
+        <v>705</v>
+      </c>
+      <c r="T5" s="25">
+        <v>15313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1457,8 +1592,20 @@
       <c r="P6" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="25">
+        <v>30</v>
+      </c>
+      <c r="R6" s="25">
+        <v>832</v>
+      </c>
+      <c r="S6" s="25">
+        <v>35</v>
+      </c>
+      <c r="T6" s="25">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1487,8 +1634,20 @@
       <c r="P7" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q7" s="25">
+        <v>2</v>
+      </c>
+      <c r="R7" s="25">
+        <v>121</v>
+      </c>
+      <c r="S7" s="25">
+        <v>12</v>
+      </c>
+      <c r="T7" s="25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1525,8 +1684,20 @@
       <c r="P8" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q8" s="25">
+        <v>190</v>
+      </c>
+      <c r="R8" s="25">
+        <v>2535</v>
+      </c>
+      <c r="S8" s="25">
+        <v>2010</v>
+      </c>
+      <c r="T8" s="25">
+        <v>14493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -1545,8 +1716,20 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="12"/>
-    </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q9" s="25">
+        <v>13</v>
+      </c>
+      <c r="R9" s="25">
+        <v>290</v>
+      </c>
+      <c r="S9" s="25">
+        <v>1</v>
+      </c>
+      <c r="T9" s="25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1587,8 +1770,20 @@
       <c r="P10" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q10" s="25">
+        <v>27</v>
+      </c>
+      <c r="R10" s="25">
+        <v>555</v>
+      </c>
+      <c r="S10" s="25">
+        <v>124</v>
+      </c>
+      <c r="T10" s="25">
+        <v>5236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1633,8 +1828,20 @@
       <c r="P11" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q11" s="25">
+        <v>106</v>
+      </c>
+      <c r="R11" s="25">
+        <v>340</v>
+      </c>
+      <c r="S11" s="25">
+        <v>309</v>
+      </c>
+      <c r="T11" s="25">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1667,8 +1874,20 @@
       <c r="P12" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q12" s="25">
+        <v>9</v>
+      </c>
+      <c r="R12" s="25">
+        <v>419</v>
+      </c>
+      <c r="S12" s="25">
+        <v>24</v>
+      </c>
+      <c r="T12" s="25">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1699,8 +1918,20 @@
       <c r="P13" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q13" s="25">
+        <v>190</v>
+      </c>
+      <c r="R13" s="25">
+        <v>3440</v>
+      </c>
+      <c r="S13" s="25">
+        <v>47</v>
+      </c>
+      <c r="T13" s="25">
+        <v>3918</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1739,8 +1970,20 @@
       <c r="P14" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q14" s="25">
+        <v>22</v>
+      </c>
+      <c r="R14" s="25">
+        <v>763</v>
+      </c>
+      <c r="S14" s="25">
+        <v>73</v>
+      </c>
+      <c r="T14" s="25">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1783,11 +2026,20 @@
       <c r="P15" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q15" s="25">
+        <v>112</v>
+      </c>
+      <c r="R15" s="25">
+        <v>1124</v>
+      </c>
+      <c r="S15" s="25">
+        <v>29</v>
+      </c>
+      <c r="T15" s="25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
@@ -1830,11 +2082,20 @@
       <c r="P16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q16" s="25">
+        <v>16</v>
+      </c>
+      <c r="R16" s="25">
+        <v>116</v>
+      </c>
+      <c r="S16" s="25">
+        <v>7</v>
+      </c>
+      <c r="T16" s="25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -1865,8 +2126,20 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="12"/>
-    </row>
-    <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q17" s="25">
+        <v>10</v>
+      </c>
+      <c r="R17" s="25">
+        <v>873</v>
+      </c>
+      <c r="S17" s="25">
+        <v>13</v>
+      </c>
+      <c r="T17" s="25">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1911,8 +2184,20 @@
       <c r="P18" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q18" s="25">
+        <v>142</v>
+      </c>
+      <c r="R18" s="25">
+        <v>2481</v>
+      </c>
+      <c r="S18" s="25">
+        <v>13</v>
+      </c>
+      <c r="T18" s="25">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -1931,8 +2216,20 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q19" s="25">
+        <v>23</v>
+      </c>
+      <c r="R19" s="25">
+        <v>1426</v>
+      </c>
+      <c r="S19" s="25">
+        <v>46</v>
+      </c>
+      <c r="T19" s="25">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
@@ -1951,8 +2248,20 @@
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q20" s="25">
+        <v>23</v>
+      </c>
+      <c r="R20" s="25">
+        <v>1498</v>
+      </c>
+      <c r="S20" s="25">
+        <v>1</v>
+      </c>
+      <c r="T20" s="25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1995,8 +2304,20 @@
       <c r="P21" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q21" s="25">
+        <v>532</v>
+      </c>
+      <c r="R21" s="25">
+        <v>1523</v>
+      </c>
+      <c r="S21" s="25">
+        <v>2008</v>
+      </c>
+      <c r="T21" s="25">
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -2043,11 +2364,20 @@
       <c r="P22" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q22" s="25">
+        <v>14002</v>
+      </c>
+      <c r="R22" s="25">
+        <v>17890</v>
+      </c>
+      <c r="S22" s="25">
+        <v>8960</v>
+      </c>
+      <c r="T22" s="25">
+        <v>19573</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
@@ -2090,8 +2420,20 @@
       <c r="P23" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q23" s="25">
+        <v>487</v>
+      </c>
+      <c r="R23" s="25">
+        <v>13845</v>
+      </c>
+      <c r="S23" s="25">
+        <v>915</v>
+      </c>
+      <c r="T23" s="25">
+        <v>19054</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
@@ -2134,8 +2476,20 @@
       <c r="P24" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q24" s="25">
+        <v>230</v>
+      </c>
+      <c r="R24" s="25">
+        <v>513</v>
+      </c>
+      <c r="S24" s="25">
+        <v>1022</v>
+      </c>
+      <c r="T24" s="25">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
@@ -2172,8 +2526,20 @@
       <c r="P25" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q25" s="25">
+        <v>1</v>
+      </c>
+      <c r="R25" s="25">
+        <v>220</v>
+      </c>
+      <c r="S25" s="25">
+        <v>0</v>
+      </c>
+      <c r="T25" s="25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
@@ -2198,8 +2564,20 @@
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="12"/>
-    </row>
-    <row r="27" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q26" s="25">
+        <v>11</v>
+      </c>
+      <c r="R26" s="25">
+        <v>368</v>
+      </c>
+      <c r="S26" s="25">
+        <v>0</v>
+      </c>
+      <c r="T26" s="25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
@@ -2240,8 +2618,20 @@
       <c r="P27" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q27" s="25">
+        <v>17</v>
+      </c>
+      <c r="R27" s="25">
+        <v>1035</v>
+      </c>
+      <c r="S27" s="25">
+        <v>4</v>
+      </c>
+      <c r="T27" s="25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -2264,11 +2654,20 @@
       <c r="P28" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q28" s="25">
+        <v>15</v>
+      </c>
+      <c r="R28" s="25">
+        <v>976</v>
+      </c>
+      <c r="S28" s="25">
+        <v>1</v>
+      </c>
+      <c r="T28" s="25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>14</v>
       </c>
@@ -2291,11 +2690,20 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="12"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q29" s="25">
+        <v>9</v>
+      </c>
+      <c r="R29" s="25">
+        <v>187</v>
+      </c>
+      <c r="S29" s="25">
+        <v>27</v>
+      </c>
+      <c r="T29" s="25">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
@@ -2318,8 +2726,20 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="12"/>
-    </row>
-    <row r="31" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q30" s="25">
+        <v>3</v>
+      </c>
+      <c r="R30" s="25">
+        <v>400</v>
+      </c>
+      <c r="S30" s="25">
+        <v>2</v>
+      </c>
+      <c r="T30" s="25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>41</v>
       </c>
@@ -2364,8 +2784,20 @@
       <c r="P31" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q31" s="25">
+        <v>379</v>
+      </c>
+      <c r="R31" s="25">
+        <v>4878</v>
+      </c>
+      <c r="S31" s="25">
+        <v>78</v>
+      </c>
+      <c r="T31" s="25">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>42</v>
       </c>
@@ -2388,8 +2820,20 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="12"/>
-    </row>
-    <row r="33" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q32" s="25">
+        <v>6</v>
+      </c>
+      <c r="R32" s="25">
+        <v>420</v>
+      </c>
+      <c r="S32" s="25">
+        <v>3</v>
+      </c>
+      <c r="T32" s="25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -2432,8 +2876,20 @@
       <c r="P33" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q33" s="25">
+        <v>253</v>
+      </c>
+      <c r="R33" s="25">
+        <v>935</v>
+      </c>
+      <c r="S33" s="25">
+        <v>56</v>
+      </c>
+      <c r="T33" s="25">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
@@ -2480,8 +2936,20 @@
       <c r="P34" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q34" s="25">
+        <v>998</v>
+      </c>
+      <c r="R34" s="25">
+        <v>1504</v>
+      </c>
+      <c r="S34" s="25">
+        <v>1087</v>
+      </c>
+      <c r="T34" s="25">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>39</v>
       </c>
@@ -2520,8 +2988,20 @@
       <c r="P35" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q35" s="25">
+        <v>877</v>
+      </c>
+      <c r="R35" s="25">
+        <v>14519</v>
+      </c>
+      <c r="S35" s="25">
+        <v>130</v>
+      </c>
+      <c r="T35" s="25">
+        <v>6942</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
@@ -2552,8 +3032,20 @@
       <c r="P36" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q36" s="25">
+        <v>206</v>
+      </c>
+      <c r="R36" s="25">
+        <v>10995</v>
+      </c>
+      <c r="S36" s="25">
+        <v>139</v>
+      </c>
+      <c r="T36" s="25">
+        <v>6594</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
@@ -2588,8 +3080,20 @@
       <c r="P37" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q37" s="25">
+        <v>3</v>
+      </c>
+      <c r="R37" s="25">
+        <v>246</v>
+      </c>
+      <c r="S37" s="25">
+        <v>4</v>
+      </c>
+      <c r="T37" s="25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
@@ -2612,8 +3116,20 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
       <c r="P38" s="12"/>
-    </row>
-    <row r="39" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q38" s="25">
+        <v>6</v>
+      </c>
+      <c r="R38" s="25">
+        <v>141</v>
+      </c>
+      <c r="S38" s="25">
+        <v>2</v>
+      </c>
+      <c r="T38" s="25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>6</v>
       </c>
@@ -2640,8 +3156,20 @@
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
       <c r="P39" s="12"/>
-    </row>
-    <row r="40" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q39" s="25">
+        <v>11</v>
+      </c>
+      <c r="R39" s="25">
+        <v>512</v>
+      </c>
+      <c r="S39" s="25">
+        <v>23</v>
+      </c>
+      <c r="T39" s="25">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>16</v>
       </c>
@@ -2660,8 +3188,20 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
       <c r="P40" s="12"/>
-    </row>
-    <row r="41" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q40" s="25">
+        <v>0</v>
+      </c>
+      <c r="R40" s="25">
+        <v>25</v>
+      </c>
+      <c r="S40" s="25">
+        <v>4</v>
+      </c>
+      <c r="T40" s="25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>12</v>
       </c>
@@ -2702,8 +3242,20 @@
       <c r="P41" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q41" s="25">
+        <v>165</v>
+      </c>
+      <c r="R41" s="25">
+        <v>2931</v>
+      </c>
+      <c r="S41" s="25">
+        <v>17</v>
+      </c>
+      <c r="T41" s="25">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>43</v>
       </c>
@@ -2734,8 +3286,20 @@
       <c r="P42" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q42" s="25">
+        <v>39</v>
+      </c>
+      <c r="R42" s="25">
+        <v>2420</v>
+      </c>
+      <c r="S42" s="25">
+        <v>18</v>
+      </c>
+      <c r="T42" s="25">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
@@ -2772,8 +3336,20 @@
       <c r="P43" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q43" s="25">
+        <v>88</v>
+      </c>
+      <c r="R43" s="25">
+        <v>5373</v>
+      </c>
+      <c r="S43" s="25">
+        <v>46</v>
+      </c>
+      <c r="T43" s="25">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>15</v>
       </c>
@@ -2814,8 +3390,20 @@
       <c r="P44" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q44" s="25">
+        <v>33</v>
+      </c>
+      <c r="R44" s="25">
+        <v>1792</v>
+      </c>
+      <c r="S44" s="25">
+        <v>1</v>
+      </c>
+      <c r="T44" s="25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>7</v>
       </c>
@@ -2852,8 +3440,20 @@
       <c r="P45" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q45" s="25">
+        <v>3</v>
+      </c>
+      <c r="R45" s="25">
+        <v>199</v>
+      </c>
+      <c r="S45" s="25">
+        <v>8</v>
+      </c>
+      <c r="T45" s="25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>22</v>
       </c>
@@ -2896,8 +3496,20 @@
       <c r="P46" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q46" s="25">
+        <v>306</v>
+      </c>
+      <c r="R46" s="25">
+        <v>621</v>
+      </c>
+      <c r="S46" s="25">
+        <v>71</v>
+      </c>
+      <c r="T46" s="25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>92</v>
       </c>
@@ -2944,8 +3556,20 @@
       <c r="P47" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q47" s="25">
+        <v>99</v>
+      </c>
+      <c r="R47" s="25">
+        <v>514</v>
+      </c>
+      <c r="S47" s="25">
+        <v>92</v>
+      </c>
+      <c r="T47" s="25">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>94</v>
       </c>
@@ -2988,8 +3612,20 @@
       <c r="P48" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q48" s="25">
+        <v>196</v>
+      </c>
+      <c r="R48" s="25">
+        <v>2612</v>
+      </c>
+      <c r="S48" s="25">
+        <v>184</v>
+      </c>
+      <c r="T48" s="25">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>96</v>
       </c>
@@ -3030,8 +3666,20 @@
       <c r="P49" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q49" s="25">
+        <v>99</v>
+      </c>
+      <c r="R49" s="25">
+        <v>565</v>
+      </c>
+      <c r="S49" s="25">
+        <v>4825</v>
+      </c>
+      <c r="T49" s="25">
+        <v>10513</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>98</v>
       </c>
@@ -3058,8 +3706,20 @@
       <c r="P50" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q50" s="25">
+        <v>6</v>
+      </c>
+      <c r="R50" s="25">
+        <v>316</v>
+      </c>
+      <c r="S50" s="25">
+        <v>25</v>
+      </c>
+      <c r="T50" s="25">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>23</v>
       </c>
@@ -3078,13 +3738,1455 @@
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="25"/>
+      <c r="S51" s="25"/>
+      <c r="T51" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:A51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="1">
+  <mergeCells count="3">
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="B1:N1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DCD287-A392-E644-8B1A-F0F16250F623}">
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>6594.3897500000003</v>
+      </c>
+      <c r="C2">
+        <v>6548.6049999999996</v>
+      </c>
+      <c r="D2">
+        <v>5107.7550000000001</v>
+      </c>
+      <c r="E2">
+        <v>8061.2089999999898</v>
+      </c>
+      <c r="F2">
+        <v>138.84314149999901</v>
+      </c>
+      <c r="G2">
+        <v>135.94099999999901</v>
+      </c>
+      <c r="H2">
+        <v>96.333519999999993</v>
+      </c>
+      <c r="I2">
+        <v>189.29794999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>42.868941999999997</v>
+      </c>
+      <c r="C3">
+        <v>37.710850000000001</v>
+      </c>
+      <c r="D3">
+        <v>24.716280000000001</v>
+      </c>
+      <c r="E3">
+        <v>75.756349999999898</v>
+      </c>
+      <c r="F3">
+        <v>1.2554264799999999</v>
+      </c>
+      <c r="G3">
+        <v>0.77146000000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.33353709999999998</v>
+      </c>
+      <c r="I3">
+        <v>3.9729424999999901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1657.1980249999999</v>
+      </c>
+      <c r="C4">
+        <v>1407.41</v>
+      </c>
+      <c r="D4">
+        <v>631.68830000000003</v>
+      </c>
+      <c r="E4">
+        <v>3670.2604999999899</v>
+      </c>
+      <c r="F4">
+        <v>1022.26444999999</v>
+      </c>
+      <c r="G4">
+        <v>875.87450000000001</v>
+      </c>
+      <c r="H4">
+        <v>219.10905</v>
+      </c>
+      <c r="I4">
+        <v>2403.1019999999899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>91.398313999999999</v>
+      </c>
+      <c r="C5">
+        <v>85.941749999999999</v>
+      </c>
+      <c r="D5">
+        <v>55.145139999999998</v>
+      </c>
+      <c r="E5">
+        <v>150.74449999999899</v>
+      </c>
+      <c r="F5">
+        <v>1.3019386199999901</v>
+      </c>
+      <c r="G5">
+        <v>0.96467899999999995</v>
+      </c>
+      <c r="H5">
+        <v>0.41218044999999998</v>
+      </c>
+      <c r="I5">
+        <v>3.2121329999999899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>434.14211499999999</v>
+      </c>
+      <c r="C6">
+        <v>385.32799999999997</v>
+      </c>
+      <c r="D6">
+        <v>197.49870000000001</v>
+      </c>
+      <c r="E6">
+        <v>791.31159999999898</v>
+      </c>
+      <c r="F6">
+        <v>70.500325000000004</v>
+      </c>
+      <c r="G6">
+        <v>54.122799999999998</v>
+      </c>
+      <c r="H6">
+        <v>23.941029999999898</v>
+      </c>
+      <c r="I6">
+        <v>153.44914999999901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>3874.7948000000001</v>
+      </c>
+      <c r="C7">
+        <v>3508.2350000000001</v>
+      </c>
+      <c r="D7">
+        <v>2287.0619999999999</v>
+      </c>
+      <c r="E7">
+        <v>6686.4520000000002</v>
+      </c>
+      <c r="F7">
+        <v>24.4758958</v>
+      </c>
+      <c r="G7">
+        <v>18.5701</v>
+      </c>
+      <c r="H7">
+        <v>8.4703944999999994</v>
+      </c>
+      <c r="I7">
+        <v>62.2378649999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>484.40420999999998</v>
+      </c>
+      <c r="C8">
+        <v>416.76499999999999</v>
+      </c>
+      <c r="D8">
+        <v>171.51900000000001</v>
+      </c>
+      <c r="E8">
+        <v>1078.4424999999901</v>
+      </c>
+      <c r="F8">
+        <v>12.249886049999899</v>
+      </c>
+      <c r="G8">
+        <v>10.9138</v>
+      </c>
+      <c r="H8">
+        <v>2.9014085000000001</v>
+      </c>
+      <c r="I8">
+        <v>29.694319999999902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1673.73044</v>
+      </c>
+      <c r="C9">
+        <v>1535.65</v>
+      </c>
+      <c r="D9">
+        <v>675.09389999999996</v>
+      </c>
+      <c r="E9">
+        <v>3146.3619999999901</v>
+      </c>
+      <c r="F9">
+        <v>1087.0228050000001</v>
+      </c>
+      <c r="G9">
+        <v>830.31199999999899</v>
+      </c>
+      <c r="H9">
+        <v>230.09039999999999</v>
+      </c>
+      <c r="I9">
+        <v>2644.4274999999898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>14493.3105</v>
+      </c>
+      <c r="C10">
+        <v>14274.25</v>
+      </c>
+      <c r="D10">
+        <v>12927.014999999999</v>
+      </c>
+      <c r="E10">
+        <v>16619.57</v>
+      </c>
+      <c r="F10">
+        <v>2009.78755</v>
+      </c>
+      <c r="G10">
+        <v>1930.11499999999</v>
+      </c>
+      <c r="H10">
+        <v>1412.3129999999901</v>
+      </c>
+      <c r="I10">
+        <v>2809.6819999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>1010.32981</v>
+      </c>
+      <c r="C11">
+        <v>1044.5150000000001</v>
+      </c>
+      <c r="D11">
+        <v>435.76015000000001</v>
+      </c>
+      <c r="E11">
+        <v>1554.681</v>
+      </c>
+      <c r="F11">
+        <v>24.682880249999901</v>
+      </c>
+      <c r="G11">
+        <v>24.02365</v>
+      </c>
+      <c r="H11">
+        <v>6.0949460000000002</v>
+      </c>
+      <c r="I11">
+        <v>47.9046599999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>161.54995600000001</v>
+      </c>
+      <c r="C12">
+        <v>149.8115</v>
+      </c>
+      <c r="D12">
+        <v>106.01835</v>
+      </c>
+      <c r="E12">
+        <v>248.555049999999</v>
+      </c>
+      <c r="F12">
+        <v>3.5292770600000001</v>
+      </c>
+      <c r="G12">
+        <v>2.7144649999999899</v>
+      </c>
+      <c r="H12">
+        <v>1.3854644999999901</v>
+      </c>
+      <c r="I12">
+        <v>8.6834669999999896</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13">
+        <v>1369.0233705000001</v>
+      </c>
+      <c r="C13">
+        <v>595.21600000000001</v>
+      </c>
+      <c r="D13">
+        <v>117.94615</v>
+      </c>
+      <c r="E13">
+        <v>5134.0739999999796</v>
+      </c>
+      <c r="F13">
+        <v>91.8249432799999</v>
+      </c>
+      <c r="G13">
+        <v>16.463850000000001</v>
+      </c>
+      <c r="H13">
+        <v>2.0359829999999999</v>
+      </c>
+      <c r="I13">
+        <v>364.828149999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>999.02944000000002</v>
+      </c>
+      <c r="C14">
+        <v>966.25350000000003</v>
+      </c>
+      <c r="D14">
+        <v>766.01099999999997</v>
+      </c>
+      <c r="E14">
+        <v>1308.6635000000001</v>
+      </c>
+      <c r="F14">
+        <v>17.296248199999901</v>
+      </c>
+      <c r="G14">
+        <v>16.408899999999999</v>
+      </c>
+      <c r="H14">
+        <v>10.364915</v>
+      </c>
+      <c r="I14">
+        <v>27.103804999999898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>363.40441900000002</v>
+      </c>
+      <c r="C15">
+        <v>242.57050000000001</v>
+      </c>
+      <c r="D15">
+        <v>58.427945000000001</v>
+      </c>
+      <c r="E15">
+        <v>1092.6085</v>
+      </c>
+      <c r="F15">
+        <v>8.4330002939999993</v>
+      </c>
+      <c r="G15">
+        <v>3.0653899999999998</v>
+      </c>
+      <c r="H15">
+        <v>0.25866665</v>
+      </c>
+      <c r="I15">
+        <v>36.8177599999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16">
+        <v>2276.4759949999998</v>
+      </c>
+      <c r="C16">
+        <v>1800.9549999999999</v>
+      </c>
+      <c r="D16">
+        <v>974.10704999999996</v>
+      </c>
+      <c r="E16">
+        <v>5376.6599999999899</v>
+      </c>
+      <c r="F16">
+        <v>183.60107499999901</v>
+      </c>
+      <c r="G16">
+        <v>146.36149999999901</v>
+      </c>
+      <c r="H16">
+        <v>57.717644999999997</v>
+      </c>
+      <c r="I16">
+        <v>404.37594999999902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>19054.222000000002</v>
+      </c>
+      <c r="C17">
+        <v>18224.95</v>
+      </c>
+      <c r="D17">
+        <v>14213.305</v>
+      </c>
+      <c r="E17">
+        <v>26208.464999999898</v>
+      </c>
+      <c r="F17">
+        <v>914.93977499999903</v>
+      </c>
+      <c r="G17">
+        <v>862.97249999999997</v>
+      </c>
+      <c r="H17">
+        <v>594.14035000000001</v>
+      </c>
+      <c r="I17">
+        <v>1426.7729999999899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>2442.0943000000002</v>
+      </c>
+      <c r="C18">
+        <v>2359.29</v>
+      </c>
+      <c r="D18">
+        <v>1851.84</v>
+      </c>
+      <c r="E18">
+        <v>3216.9569999999999</v>
+      </c>
+      <c r="F18">
+        <v>45.585711499999903</v>
+      </c>
+      <c r="G18">
+        <v>43.184150000000002</v>
+      </c>
+      <c r="H18">
+        <v>29.95363</v>
+      </c>
+      <c r="I18">
+        <v>64.334984999999904</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>154.86132115000001</v>
+      </c>
+      <c r="C19">
+        <v>70.812550000000002</v>
+      </c>
+      <c r="D19">
+        <v>8.5686025000000008</v>
+      </c>
+      <c r="E19">
+        <v>521.00949999999796</v>
+      </c>
+      <c r="F19">
+        <v>1.8021787123499899</v>
+      </c>
+      <c r="G19">
+        <v>0.52349849999999998</v>
+      </c>
+      <c r="H19">
+        <v>3.5118269999999903E-2</v>
+      </c>
+      <c r="I19">
+        <v>7.266553</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>223.0963155</v>
+      </c>
+      <c r="C20">
+        <v>200.94649999999999</v>
+      </c>
+      <c r="D20">
+        <v>93.675385000000006</v>
+      </c>
+      <c r="E20">
+        <v>457.18674999999899</v>
+      </c>
+      <c r="F20">
+        <v>1.5724151549999901</v>
+      </c>
+      <c r="G20">
+        <v>1.281085</v>
+      </c>
+      <c r="H20">
+        <v>0.31905014999999998</v>
+      </c>
+      <c r="I20">
+        <v>3.5449014999999902</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3604.9456930000001</v>
+      </c>
+      <c r="C21">
+        <v>2545.2150000000001</v>
+      </c>
+      <c r="D21">
+        <v>285.77600000000001</v>
+      </c>
+      <c r="E21">
+        <v>10276.969999999899</v>
+      </c>
+      <c r="F21">
+        <v>2008.4003507999901</v>
+      </c>
+      <c r="G21">
+        <v>1158.7550000000001</v>
+      </c>
+      <c r="H21">
+        <v>49.081090000000003</v>
+      </c>
+      <c r="I21">
+        <v>6410.4089999999896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22">
+        <v>10512.696355</v>
+      </c>
+      <c r="C22">
+        <v>9904.19</v>
+      </c>
+      <c r="D22">
+        <v>767.92904999999996</v>
+      </c>
+      <c r="E22">
+        <v>21684.709999999901</v>
+      </c>
+      <c r="F22">
+        <v>4825.4675139499996</v>
+      </c>
+      <c r="G22">
+        <v>3838.67</v>
+      </c>
+      <c r="H22">
+        <v>66.606380000000001</v>
+      </c>
+      <c r="I22">
+        <v>11411.3299999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>43.957536294999997</v>
+      </c>
+      <c r="C23">
+        <v>26.158300000000001</v>
+      </c>
+      <c r="D23">
+        <v>3.3463935</v>
+      </c>
+      <c r="E23">
+        <v>143.13629999999901</v>
+      </c>
+      <c r="F23">
+        <v>7.1506017267950002</v>
+      </c>
+      <c r="G23">
+        <v>0.73348899999999995</v>
+      </c>
+      <c r="H23">
+        <v>8.9765499999999998E-3</v>
+      </c>
+      <c r="I23">
+        <v>24.718299999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>14.440093750000001</v>
+      </c>
+      <c r="C24">
+        <v>12.9521</v>
+      </c>
+      <c r="D24">
+        <v>7.0149759999999999</v>
+      </c>
+      <c r="E24">
+        <v>26.876035000000002</v>
+      </c>
+      <c r="F24">
+        <v>0.125575533749999</v>
+      </c>
+      <c r="G24">
+        <v>9.3662449999999994E-2</v>
+      </c>
+      <c r="H24">
+        <v>1.7207984999999999E-2</v>
+      </c>
+      <c r="I24">
+        <v>0.32412069999999898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>18.9527681</v>
+      </c>
+      <c r="C25">
+        <v>15.11425</v>
+      </c>
+      <c r="D25">
+        <v>7.2067509999999997</v>
+      </c>
+      <c r="E25">
+        <v>41.666829999999898</v>
+      </c>
+      <c r="F25">
+        <v>0.12180775275</v>
+      </c>
+      <c r="G25">
+        <v>6.4500649999999896E-2</v>
+      </c>
+      <c r="H25">
+        <v>1.6647240000000001E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.41718079999999902</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>137.3818325</v>
+      </c>
+      <c r="C26">
+        <v>120.279</v>
+      </c>
+      <c r="D26">
+        <v>71.107939999999999</v>
+      </c>
+      <c r="E26">
+        <v>248.95934999999901</v>
+      </c>
+      <c r="F26">
+        <v>1.496870055</v>
+      </c>
+      <c r="G26">
+        <v>1.0718749999999999</v>
+      </c>
+      <c r="H26">
+        <v>0.44422584999999998</v>
+      </c>
+      <c r="I26">
+        <v>3.3145119999999899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2260.0578</v>
+      </c>
+      <c r="C27">
+        <v>2121.89</v>
+      </c>
+      <c r="D27">
+        <v>1408.8844999999999</v>
+      </c>
+      <c r="E27">
+        <v>3538.8779999999902</v>
+      </c>
+      <c r="F27">
+        <v>45.535838999999903</v>
+      </c>
+      <c r="G27">
+        <v>39.748849999999997</v>
+      </c>
+      <c r="H27">
+        <v>21.566739999999999</v>
+      </c>
+      <c r="I27">
+        <v>86.841389999999905</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>1744.3933500000001</v>
+      </c>
+      <c r="C28">
+        <v>1690.1</v>
+      </c>
+      <c r="D28">
+        <v>1272.597</v>
+      </c>
+      <c r="E28">
+        <v>2200.6199999999899</v>
+      </c>
+      <c r="F28">
+        <v>26.887368500000001</v>
+      </c>
+      <c r="G28">
+        <v>24.34975</v>
+      </c>
+      <c r="H28">
+        <v>14.515755</v>
+      </c>
+      <c r="I28">
+        <v>40.942684999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>1255.68397</v>
+      </c>
+      <c r="C29">
+        <v>1085.7650000000001</v>
+      </c>
+      <c r="D29">
+        <v>548.26289999999995</v>
+      </c>
+      <c r="E29">
+        <v>2462.1279999999902</v>
+      </c>
+      <c r="F29">
+        <v>12.6746033499999</v>
+      </c>
+      <c r="G29">
+        <v>9.0519149999999993</v>
+      </c>
+      <c r="H29">
+        <v>3.9449550000000002</v>
+      </c>
+      <c r="I29">
+        <v>32.328979999999902</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>37367.705499999996</v>
+      </c>
+      <c r="C30">
+        <v>36015.800000000003</v>
+      </c>
+      <c r="D30">
+        <v>28117.904999999999</v>
+      </c>
+      <c r="E30">
+        <v>52325.53</v>
+      </c>
+      <c r="F30">
+        <v>2040.88941999999</v>
+      </c>
+      <c r="G30">
+        <v>1911.02</v>
+      </c>
+      <c r="H30">
+        <v>1372.9349999999999</v>
+      </c>
+      <c r="I30">
+        <v>3348.9724999999899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>1072.41842</v>
+      </c>
+      <c r="C31">
+        <v>1031.3050000000001</v>
+      </c>
+      <c r="D31">
+        <v>752.04364999999996</v>
+      </c>
+      <c r="E31">
+        <v>1682.07349999999</v>
+      </c>
+      <c r="F31">
+        <v>18.141263949999999</v>
+      </c>
+      <c r="G31">
+        <v>16.007750000000001</v>
+      </c>
+      <c r="H31">
+        <v>9.2926359999999999</v>
+      </c>
+      <c r="I31">
+        <v>33.879729999999903</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>678.93374500000004</v>
+      </c>
+      <c r="C32">
+        <v>659.274</v>
+      </c>
+      <c r="D32">
+        <v>331.97140000000002</v>
+      </c>
+      <c r="E32">
+        <v>1089.7945</v>
+      </c>
+      <c r="F32">
+        <v>308.95758049999898</v>
+      </c>
+      <c r="G32">
+        <v>303.80599999999998</v>
+      </c>
+      <c r="H32">
+        <v>107.805599999999</v>
+      </c>
+      <c r="I32">
+        <v>538.98219999999901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>900.48133499999994</v>
+      </c>
+      <c r="C33">
+        <v>869.14499999999998</v>
+      </c>
+      <c r="D33">
+        <v>420.02224999999999</v>
+      </c>
+      <c r="E33">
+        <v>1536.0899999999899</v>
+      </c>
+      <c r="F33">
+        <v>28.817172449999902</v>
+      </c>
+      <c r="G33">
+        <v>24.54965</v>
+      </c>
+      <c r="H33">
+        <v>7.1268349999999998</v>
+      </c>
+      <c r="I33">
+        <v>63.336574999999897</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>751.27615000000003</v>
+      </c>
+      <c r="C34">
+        <v>655.77599999999995</v>
+      </c>
+      <c r="D34">
+        <v>378.95440000000002</v>
+      </c>
+      <c r="E34">
+        <v>1393.55899999999</v>
+      </c>
+      <c r="F34">
+        <v>13.3701050499999</v>
+      </c>
+      <c r="G34">
+        <v>9.1934500000000003</v>
+      </c>
+      <c r="H34">
+        <v>3.9623794999999999</v>
+      </c>
+      <c r="I34">
+        <v>31.618084999999901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>15313.369549999999</v>
+      </c>
+      <c r="C35">
+        <v>14497.3</v>
+      </c>
+      <c r="D35">
+        <v>10479.834999999999</v>
+      </c>
+      <c r="E35">
+        <v>23264.63</v>
+      </c>
+      <c r="F35">
+        <v>704.69540500000005</v>
+      </c>
+      <c r="G35">
+        <v>635.46900000000005</v>
+      </c>
+      <c r="H35">
+        <v>381.01864999999998</v>
+      </c>
+      <c r="I35">
+        <v>1290.7159999999899</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>6942.1082500000002</v>
+      </c>
+      <c r="C36">
+        <v>6767.7449999999999</v>
+      </c>
+      <c r="D36">
+        <v>5065.4089999999997</v>
+      </c>
+      <c r="E36">
+        <v>9415.7445000000007</v>
+      </c>
+      <c r="F36">
+        <v>130.28793199999899</v>
+      </c>
+      <c r="G36">
+        <v>122.762</v>
+      </c>
+      <c r="H36">
+        <v>83.624054999999998</v>
+      </c>
+      <c r="I36">
+        <v>196.20684999999901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>329.52892300000002</v>
+      </c>
+      <c r="C37">
+        <v>234.56049999999999</v>
+      </c>
+      <c r="D37">
+        <v>33.843854999999998</v>
+      </c>
+      <c r="E37">
+        <v>1085.0474999999999</v>
+      </c>
+      <c r="F37">
+        <v>4.3258210399999903</v>
+      </c>
+      <c r="G37">
+        <v>2.4145199999999898</v>
+      </c>
+      <c r="H37">
+        <v>0.2550366</v>
+      </c>
+      <c r="I37">
+        <v>17.2635299999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>5236.1251499999998</v>
+      </c>
+      <c r="C38">
+        <v>4845.5050000000001</v>
+      </c>
+      <c r="D38">
+        <v>2868.4115000000002</v>
+      </c>
+      <c r="E38">
+        <v>8582.1284999999898</v>
+      </c>
+      <c r="F38">
+        <v>124.39123149999899</v>
+      </c>
+      <c r="G38">
+        <v>105.71899999999999</v>
+      </c>
+      <c r="H38">
+        <v>47.08746</v>
+      </c>
+      <c r="I38">
+        <v>262.03049999999899</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>751.55859499999997</v>
+      </c>
+      <c r="C39">
+        <v>666.98149999999998</v>
+      </c>
+      <c r="D39">
+        <v>311.75225</v>
+      </c>
+      <c r="E39">
+        <v>1442.49449999999</v>
+      </c>
+      <c r="F39">
+        <v>35.436678800000003</v>
+      </c>
+      <c r="G39">
+        <v>25.706849999999999</v>
+      </c>
+      <c r="H39">
+        <v>5.375515</v>
+      </c>
+      <c r="I39">
+        <v>94.997159999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>77.677379999999999</v>
+      </c>
+      <c r="C40">
+        <v>76.434550000000002</v>
+      </c>
+      <c r="D40">
+        <v>47.604965</v>
+      </c>
+      <c r="E40">
+        <v>112.240999999999</v>
+      </c>
+      <c r="F40">
+        <v>1.13111936499999</v>
+      </c>
+      <c r="G40">
+        <v>1.0425549999999999</v>
+      </c>
+      <c r="H40">
+        <v>0.38209009999999899</v>
+      </c>
+      <c r="I40">
+        <v>2.26315449999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>19573.240399999999</v>
+      </c>
+      <c r="C41">
+        <v>15532.65</v>
+      </c>
+      <c r="D41">
+        <v>8614.9604999999992</v>
+      </c>
+      <c r="E41">
+        <v>42784.78</v>
+      </c>
+      <c r="F41">
+        <v>8959.9521999999906</v>
+      </c>
+      <c r="G41">
+        <v>7241.86</v>
+      </c>
+      <c r="H41">
+        <v>3865.5564999999901</v>
+      </c>
+      <c r="I41">
+        <v>18490.084999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <v>3917.5972999999999</v>
+      </c>
+      <c r="C42">
+        <v>3587.67</v>
+      </c>
+      <c r="D42">
+        <v>2588.9475000000002</v>
+      </c>
+      <c r="E42">
+        <v>5958.7614999999896</v>
+      </c>
+      <c r="F42">
+        <v>46.5448065</v>
+      </c>
+      <c r="G42">
+        <v>43.046849999999999</v>
+      </c>
+      <c r="H42">
+        <v>18.013549999999999</v>
+      </c>
+      <c r="I42">
+        <v>86.257574999999903</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>177.82422299999999</v>
+      </c>
+      <c r="C43">
+        <v>140.82050000000001</v>
+      </c>
+      <c r="D43">
+        <v>81.562579999999997</v>
+      </c>
+      <c r="E43">
+        <v>384.22469999999902</v>
+      </c>
+      <c r="F43">
+        <v>2.6706287899999999</v>
+      </c>
+      <c r="G43">
+        <v>1.55871</v>
+      </c>
+      <c r="H43">
+        <v>0.59362369999999998</v>
+      </c>
+      <c r="I43">
+        <v>8.1183099999999797</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>162.78233832699999</v>
+      </c>
+      <c r="C44">
+        <v>26.83175</v>
+      </c>
+      <c r="D44">
+        <v>1.4188419999999999</v>
+      </c>
+      <c r="E44">
+        <v>594.38369999999895</v>
+      </c>
+      <c r="F44">
+        <v>3.7397955902149498</v>
+      </c>
+      <c r="G44">
+        <v>0.10244159999999999</v>
+      </c>
+      <c r="H44">
+        <v>2.4317505000000001E-4</v>
+      </c>
+      <c r="I44">
+        <v>11.085529999999901</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>2811.1804999999999</v>
+      </c>
+      <c r="C45">
+        <v>2772.855</v>
+      </c>
+      <c r="D45">
+        <v>1481.3</v>
+      </c>
+      <c r="E45">
+        <v>3979.6869999999899</v>
+      </c>
+      <c r="F45">
+        <v>77.790679499999996</v>
+      </c>
+      <c r="G45">
+        <v>74.312150000000003</v>
+      </c>
+      <c r="H45">
+        <v>27.76023</v>
+      </c>
+      <c r="I45">
+        <v>131.53924999999899</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46">
+        <v>23601.115000000002</v>
+      </c>
+      <c r="C46">
+        <v>22546.400000000001</v>
+      </c>
+      <c r="D46">
+        <v>18530.544999999998</v>
+      </c>
+      <c r="E46">
+        <v>32001.624999999902</v>
+      </c>
+      <c r="F46">
+        <v>682.14216499999895</v>
+      </c>
+      <c r="G46">
+        <v>647.3845</v>
+      </c>
+      <c r="H46">
+        <v>488.38220000000001</v>
+      </c>
+      <c r="I46">
+        <v>966.61484999999902</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>863.87073999999996</v>
+      </c>
+      <c r="C47">
+        <v>789.01149999999996</v>
+      </c>
+      <c r="D47">
+        <v>393.26145000000002</v>
+      </c>
+      <c r="E47">
+        <v>1513.56699999999</v>
+      </c>
+      <c r="F47">
+        <v>22.783891399999899</v>
+      </c>
+      <c r="G47">
+        <v>18.55125</v>
+      </c>
+      <c r="H47">
+        <v>6.0799325</v>
+      </c>
+      <c r="I47">
+        <v>49.19988</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>1587.4422549999999</v>
+      </c>
+      <c r="C48">
+        <v>1499.2550000000001</v>
+      </c>
+      <c r="D48">
+        <v>950.36284999999998</v>
+      </c>
+      <c r="E48">
+        <v>2414.8249999999898</v>
+      </c>
+      <c r="F48">
+        <v>72.7900309999999</v>
+      </c>
+      <c r="G48">
+        <v>66.304649999999995</v>
+      </c>
+      <c r="H48">
+        <v>34.287480000000002</v>
+      </c>
+      <c r="I48">
+        <v>136.64474999999899</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49">
+        <v>669.22999500000003</v>
+      </c>
+      <c r="C49">
+        <v>631.78549999999996</v>
+      </c>
+      <c r="D49">
+        <v>201.78030000000001</v>
+      </c>
+      <c r="E49">
+        <v>1249.68649999999</v>
+      </c>
+      <c r="F49">
+        <v>55.580616299999903</v>
+      </c>
+      <c r="G49">
+        <v>45.631549999999997</v>
+      </c>
+      <c r="H49">
+        <v>5.0023249999999999</v>
+      </c>
+      <c r="I49">
+        <v>147.1909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add loss model data and comparison plots
</commit_message>
<xml_diff>
--- a/loss_data/selected_damaging_events/losses_selected_damaging_events.xlsx
+++ b/loss_data/selected_damaging_events/losses_selected_damaging_events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_scenario_tests/loss_data/selected_damaging_events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD295FD-52FE-F547-A354-BF51953348C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C36AAF6-71E8-D34B-8CE2-831D3D695B5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -361,9 +361,6 @@
     <t>fatality_95</t>
   </si>
   <si>
-    <t>Total Mean Damages ($M)</t>
-  </si>
-  <si>
     <t>Total Mean Deaths</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>ESRM20 - ShakeMaps</t>
+  </si>
+  <si>
+    <t>Total Mean Damages (EUR M)</t>
   </si>
 </sst>
 </file>
@@ -755,15 +755,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -775,6 +766,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1300,7 +1300,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,38 +1320,38 @@
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="24.5" customWidth="1"/>
     <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="19"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="R1" s="24"/>
+      <c r="S1" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" s="27"/>
+      <c r="T1" s="24"/>
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
@@ -1402,17 +1402,17 @@
       <c r="P2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="R2" s="24" t="s">
+      <c r="Q2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="S2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="T2" s="24" t="s">
+      <c r="R2" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="20" t="s">
         <v>110</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1454,16 +1454,16 @@
       <c r="P3" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="22">
         <v>857</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3" s="22">
         <v>18760</v>
       </c>
-      <c r="S3" s="25">
+      <c r="S3" s="22">
         <v>682</v>
       </c>
-      <c r="T3" s="25">
+      <c r="T3" s="22">
         <v>23601</v>
       </c>
     </row>
@@ -1508,16 +1508,16 @@
       <c r="P4" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="22">
         <v>195</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="22">
         <v>1880</v>
       </c>
-      <c r="S4" s="25">
+      <c r="S4" s="22">
         <v>2041</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="22">
         <v>37368</v>
       </c>
     </row>
@@ -1540,16 +1540,16 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="12"/>
-      <c r="Q5" s="25">
+      <c r="Q5" s="22">
         <v>228</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5" s="22">
         <v>2552</v>
       </c>
-      <c r="S5" s="25">
+      <c r="S5" s="22">
         <v>705</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="22">
         <v>15313</v>
       </c>
     </row>
@@ -1592,16 +1592,16 @@
       <c r="P6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="22">
         <v>30</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="22">
         <v>832</v>
       </c>
-      <c r="S6" s="25">
+      <c r="S6" s="22">
         <v>35</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6" s="22">
         <v>752</v>
       </c>
     </row>
@@ -1634,16 +1634,16 @@
       <c r="P7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="22">
         <v>2</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="22">
         <v>121</v>
       </c>
-      <c r="S7" s="25">
+      <c r="S7" s="22">
         <v>12</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="22">
         <v>484</v>
       </c>
     </row>
@@ -1684,16 +1684,16 @@
       <c r="P8" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8" s="22">
         <v>190</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="22">
         <v>2535</v>
       </c>
-      <c r="S8" s="25">
+      <c r="S8" s="22">
         <v>2010</v>
       </c>
-      <c r="T8" s="25">
+      <c r="T8" s="22">
         <v>14493</v>
       </c>
     </row>
@@ -1716,16 +1716,16 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="12"/>
-      <c r="Q9" s="25">
+      <c r="Q9" s="22">
         <v>13</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="22">
         <v>290</v>
       </c>
-      <c r="S9" s="25">
+      <c r="S9" s="22">
         <v>1</v>
       </c>
-      <c r="T9" s="25">
+      <c r="T9" s="22">
         <v>43</v>
       </c>
     </row>
@@ -1770,16 +1770,16 @@
       <c r="P10" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="22">
         <v>27</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="22">
         <v>555</v>
       </c>
-      <c r="S10" s="25">
+      <c r="S10" s="22">
         <v>124</v>
       </c>
-      <c r="T10" s="25">
+      <c r="T10" s="22">
         <v>5236</v>
       </c>
     </row>
@@ -1828,16 +1828,16 @@
       <c r="P11" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q11" s="25">
+      <c r="Q11" s="22">
         <v>106</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11" s="22">
         <v>340</v>
       </c>
-      <c r="S11" s="25">
+      <c r="S11" s="22">
         <v>309</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11" s="22">
         <v>679</v>
       </c>
     </row>
@@ -1874,16 +1874,16 @@
       <c r="P12" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="22">
         <v>9</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="22">
         <v>419</v>
       </c>
-      <c r="S12" s="25">
+      <c r="S12" s="22">
         <v>24</v>
       </c>
-      <c r="T12" s="25">
+      <c r="T12" s="22">
         <v>3875</v>
       </c>
     </row>
@@ -1918,16 +1918,16 @@
       <c r="P13" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="22">
         <v>190</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="22">
         <v>3440</v>
       </c>
-      <c r="S13" s="25">
+      <c r="S13" s="22">
         <v>47</v>
       </c>
-      <c r="T13" s="25">
+      <c r="T13" s="22">
         <v>3918</v>
       </c>
     </row>
@@ -1970,16 +1970,16 @@
       <c r="P14" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14" s="22">
         <v>22</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="22">
         <v>763</v>
       </c>
-      <c r="S14" s="25">
+      <c r="S14" s="22">
         <v>73</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14" s="22">
         <v>1587</v>
       </c>
     </row>
@@ -2026,16 +2026,16 @@
       <c r="P15" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="22">
         <v>112</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="22">
         <v>1124</v>
       </c>
-      <c r="S15" s="25">
+      <c r="S15" s="22">
         <v>29</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T15" s="22">
         <v>900</v>
       </c>
     </row>
@@ -2082,16 +2082,16 @@
       <c r="P16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="22">
         <v>16</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16" s="22">
         <v>116</v>
       </c>
-      <c r="S16" s="25">
+      <c r="S16" s="22">
         <v>7</v>
       </c>
-      <c r="T16" s="25">
+      <c r="T16" s="22">
         <v>44</v>
       </c>
     </row>
@@ -2126,16 +2126,16 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="12"/>
-      <c r="Q17" s="25">
+      <c r="Q17" s="22">
         <v>10</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="22">
         <v>873</v>
       </c>
-      <c r="S17" s="25">
+      <c r="S17" s="22">
         <v>13</v>
       </c>
-      <c r="T17" s="25">
+      <c r="T17" s="22">
         <v>1256</v>
       </c>
     </row>
@@ -2184,16 +2184,16 @@
       <c r="P18" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="22">
         <v>142</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="22">
         <v>2481</v>
       </c>
-      <c r="S18" s="25">
+      <c r="S18" s="22">
         <v>13</v>
       </c>
-      <c r="T18" s="25">
+      <c r="T18" s="22">
         <v>751</v>
       </c>
     </row>
@@ -2216,16 +2216,16 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="12"/>
-      <c r="Q19" s="25">
+      <c r="Q19" s="22">
         <v>23</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="22">
         <v>1426</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19" s="22">
         <v>46</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19" s="22">
         <v>2260</v>
       </c>
     </row>
@@ -2248,16 +2248,16 @@
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="25">
+      <c r="Q20" s="22">
         <v>23</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="22">
         <v>1498</v>
       </c>
-      <c r="S20" s="25">
+      <c r="S20" s="22">
         <v>1</v>
       </c>
-      <c r="T20" s="25">
+      <c r="T20" s="22">
         <v>137</v>
       </c>
     </row>
@@ -2304,16 +2304,16 @@
       <c r="P21" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q21" s="25">
+      <c r="Q21" s="22">
         <v>532</v>
       </c>
-      <c r="R21" s="25">
+      <c r="R21" s="22">
         <v>1523</v>
       </c>
-      <c r="S21" s="25">
+      <c r="S21" s="22">
         <v>2008</v>
       </c>
-      <c r="T21" s="25">
+      <c r="T21" s="22">
         <v>3605</v>
       </c>
     </row>
@@ -2364,16 +2364,16 @@
       <c r="P22" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q22" s="25">
+      <c r="Q22" s="22">
         <v>14002</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22" s="22">
         <v>17890</v>
       </c>
-      <c r="S22" s="25">
+      <c r="S22" s="22">
         <v>8960</v>
       </c>
-      <c r="T22" s="25">
+      <c r="T22" s="22">
         <v>19573</v>
       </c>
     </row>
@@ -2420,16 +2420,16 @@
       <c r="P23" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q23" s="25">
+      <c r="Q23" s="22">
         <v>487</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23" s="22">
         <v>13845</v>
       </c>
-      <c r="S23" s="25">
+      <c r="S23" s="22">
         <v>915</v>
       </c>
-      <c r="T23" s="25">
+      <c r="T23" s="22">
         <v>19054</v>
       </c>
     </row>
@@ -2476,16 +2476,16 @@
       <c r="P24" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q24" s="25">
+      <c r="Q24" s="22">
         <v>230</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R24" s="22">
         <v>513</v>
       </c>
-      <c r="S24" s="25">
+      <c r="S24" s="22">
         <v>1022</v>
       </c>
-      <c r="T24" s="25">
+      <c r="T24" s="22">
         <v>1657</v>
       </c>
     </row>
@@ -2526,16 +2526,16 @@
       <c r="P25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q25" s="25">
+      <c r="Q25" s="22">
         <v>1</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25" s="22">
         <v>220</v>
       </c>
-      <c r="S25" s="25">
+      <c r="S25" s="22">
         <v>0</v>
       </c>
-      <c r="T25" s="25">
+      <c r="T25" s="22">
         <v>14</v>
       </c>
     </row>
@@ -2564,16 +2564,16 @@
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="12"/>
-      <c r="Q26" s="25">
+      <c r="Q26" s="22">
         <v>11</v>
       </c>
-      <c r="R26" s="25">
+      <c r="R26" s="22">
         <v>368</v>
       </c>
-      <c r="S26" s="25">
+      <c r="S26" s="22">
         <v>0</v>
       </c>
-      <c r="T26" s="25">
+      <c r="T26" s="22">
         <v>19</v>
       </c>
     </row>
@@ -2618,16 +2618,16 @@
       <c r="P27" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q27" s="25">
+      <c r="Q27" s="22">
         <v>17</v>
       </c>
-      <c r="R27" s="25">
+      <c r="R27" s="22">
         <v>1035</v>
       </c>
-      <c r="S27" s="25">
+      <c r="S27" s="22">
         <v>4</v>
       </c>
-      <c r="T27" s="25">
+      <c r="T27" s="22">
         <v>162</v>
       </c>
     </row>
@@ -2654,16 +2654,16 @@
       <c r="P28" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q28" s="25">
+      <c r="Q28" s="22">
         <v>15</v>
       </c>
-      <c r="R28" s="25">
+      <c r="R28" s="22">
         <v>976</v>
       </c>
-      <c r="S28" s="25">
+      <c r="S28" s="22">
         <v>1</v>
       </c>
-      <c r="T28" s="25">
+      <c r="T28" s="22">
         <v>78</v>
       </c>
     </row>
@@ -2690,16 +2690,16 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="12"/>
-      <c r="Q29" s="25">
+      <c r="Q29" s="22">
         <v>9</v>
       </c>
-      <c r="R29" s="25">
+      <c r="R29" s="22">
         <v>187</v>
       </c>
-      <c r="S29" s="25">
+      <c r="S29" s="22">
         <v>27</v>
       </c>
-      <c r="T29" s="25">
+      <c r="T29" s="22">
         <v>1744</v>
       </c>
     </row>
@@ -2726,16 +2726,16 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="12"/>
-      <c r="Q30" s="25">
+      <c r="Q30" s="22">
         <v>3</v>
       </c>
-      <c r="R30" s="25">
+      <c r="R30" s="22">
         <v>400</v>
       </c>
-      <c r="S30" s="25">
+      <c r="S30" s="22">
         <v>2</v>
       </c>
-      <c r="T30" s="25">
+      <c r="T30" s="22">
         <v>223</v>
       </c>
     </row>
@@ -2784,16 +2784,16 @@
       <c r="P31" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q31" s="25">
+      <c r="Q31" s="22">
         <v>379</v>
       </c>
-      <c r="R31" s="25">
+      <c r="R31" s="22">
         <v>4878</v>
       </c>
-      <c r="S31" s="25">
+      <c r="S31" s="22">
         <v>78</v>
       </c>
-      <c r="T31" s="25">
+      <c r="T31" s="22">
         <v>2811</v>
       </c>
     </row>
@@ -2820,16 +2820,16 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="12"/>
-      <c r="Q32" s="25">
+      <c r="Q32" s="22">
         <v>6</v>
       </c>
-      <c r="R32" s="25">
+      <c r="R32" s="22">
         <v>420</v>
       </c>
-      <c r="S32" s="25">
+      <c r="S32" s="22">
         <v>3</v>
       </c>
-      <c r="T32" s="25">
+      <c r="T32" s="22">
         <v>178</v>
       </c>
     </row>
@@ -2876,16 +2876,16 @@
       <c r="P33" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q33" s="25">
+      <c r="Q33" s="22">
         <v>253</v>
       </c>
-      <c r="R33" s="25">
+      <c r="R33" s="22">
         <v>935</v>
       </c>
-      <c r="S33" s="25">
+      <c r="S33" s="22">
         <v>56</v>
       </c>
-      <c r="T33" s="25">
+      <c r="T33" s="22">
         <v>669</v>
       </c>
     </row>
@@ -2936,16 +2936,16 @@
       <c r="P34" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q34" s="25">
+      <c r="Q34" s="22">
         <v>998</v>
       </c>
-      <c r="R34" s="25">
+      <c r="R34" s="22">
         <v>1504</v>
       </c>
-      <c r="S34" s="25">
+      <c r="S34" s="22">
         <v>1087</v>
       </c>
-      <c r="T34" s="25">
+      <c r="T34" s="22">
         <v>1674</v>
       </c>
     </row>
@@ -2988,16 +2988,16 @@
       <c r="P35" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q35" s="25">
+      <c r="Q35" s="22">
         <v>877</v>
       </c>
-      <c r="R35" s="25">
+      <c r="R35" s="22">
         <v>14519</v>
       </c>
-      <c r="S35" s="25">
+      <c r="S35" s="22">
         <v>130</v>
       </c>
-      <c r="T35" s="25">
+      <c r="T35" s="22">
         <v>6942</v>
       </c>
     </row>
@@ -3032,16 +3032,16 @@
       <c r="P36" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q36" s="25">
+      <c r="Q36" s="22">
         <v>206</v>
       </c>
-      <c r="R36" s="25">
+      <c r="R36" s="22">
         <v>10995</v>
       </c>
-      <c r="S36" s="25">
+      <c r="S36" s="22">
         <v>139</v>
       </c>
-      <c r="T36" s="25">
+      <c r="T36" s="22">
         <v>6594</v>
       </c>
     </row>
@@ -3080,16 +3080,16 @@
       <c r="P37" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q37" s="25">
+      <c r="Q37" s="22">
         <v>3</v>
       </c>
-      <c r="R37" s="25">
+      <c r="R37" s="22">
         <v>246</v>
       </c>
-      <c r="S37" s="25">
+      <c r="S37" s="22">
         <v>4</v>
       </c>
-      <c r="T37" s="25">
+      <c r="T37" s="22">
         <v>330</v>
       </c>
     </row>
@@ -3116,16 +3116,16 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
       <c r="P38" s="12"/>
-      <c r="Q38" s="25">
+      <c r="Q38" s="22">
         <v>6</v>
       </c>
-      <c r="R38" s="25">
+      <c r="R38" s="22">
         <v>141</v>
       </c>
-      <c r="S38" s="25">
+      <c r="S38" s="22">
         <v>2</v>
       </c>
-      <c r="T38" s="25">
+      <c r="T38" s="22">
         <v>155</v>
       </c>
     </row>
@@ -3156,16 +3156,16 @@
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
       <c r="P39" s="12"/>
-      <c r="Q39" s="25">
+      <c r="Q39" s="22">
         <v>11</v>
       </c>
-      <c r="R39" s="25">
+      <c r="R39" s="22">
         <v>512</v>
       </c>
-      <c r="S39" s="25">
+      <c r="S39" s="22">
         <v>23</v>
       </c>
-      <c r="T39" s="25">
+      <c r="T39" s="22">
         <v>864</v>
       </c>
     </row>
@@ -3188,16 +3188,16 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
       <c r="P40" s="12"/>
-      <c r="Q40" s="25">
+      <c r="Q40" s="22">
         <v>0</v>
       </c>
-      <c r="R40" s="25">
+      <c r="R40" s="22">
         <v>25</v>
       </c>
-      <c r="S40" s="25">
+      <c r="S40" s="22">
         <v>4</v>
       </c>
-      <c r="T40" s="25">
+      <c r="T40" s="22">
         <v>163</v>
       </c>
     </row>
@@ -3242,16 +3242,16 @@
       <c r="P41" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q41" s="25">
+      <c r="Q41" s="22">
         <v>165</v>
       </c>
-      <c r="R41" s="25">
+      <c r="R41" s="22">
         <v>2931</v>
       </c>
-      <c r="S41" s="25">
+      <c r="S41" s="22">
         <v>17</v>
       </c>
-      <c r="T41" s="25">
+      <c r="T41" s="22">
         <v>999</v>
       </c>
     </row>
@@ -3286,16 +3286,16 @@
       <c r="P42" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q42" s="25">
+      <c r="Q42" s="22">
         <v>39</v>
       </c>
-      <c r="R42" s="25">
+      <c r="R42" s="22">
         <v>2420</v>
       </c>
-      <c r="S42" s="25">
+      <c r="S42" s="22">
         <v>18</v>
       </c>
-      <c r="T42" s="25">
+      <c r="T42" s="22">
         <v>1072</v>
       </c>
     </row>
@@ -3336,16 +3336,16 @@
       <c r="P43" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q43" s="25">
+      <c r="Q43" s="22">
         <v>88</v>
       </c>
-      <c r="R43" s="25">
+      <c r="R43" s="22">
         <v>5373</v>
       </c>
-      <c r="S43" s="25">
+      <c r="S43" s="22">
         <v>46</v>
       </c>
-      <c r="T43" s="25">
+      <c r="T43" s="22">
         <v>2442</v>
       </c>
     </row>
@@ -3390,16 +3390,16 @@
       <c r="P44" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q44" s="25">
+      <c r="Q44" s="22">
         <v>33</v>
       </c>
-      <c r="R44" s="25">
+      <c r="R44" s="22">
         <v>1792</v>
       </c>
-      <c r="S44" s="25">
+      <c r="S44" s="22">
         <v>1</v>
       </c>
-      <c r="T44" s="25">
+      <c r="T44" s="22">
         <v>91</v>
       </c>
     </row>
@@ -3440,16 +3440,16 @@
       <c r="P45" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q45" s="25">
+      <c r="Q45" s="22">
         <v>3</v>
       </c>
-      <c r="R45" s="25">
+      <c r="R45" s="22">
         <v>199</v>
       </c>
-      <c r="S45" s="25">
+      <c r="S45" s="22">
         <v>8</v>
       </c>
-      <c r="T45" s="25">
+      <c r="T45" s="22">
         <v>363</v>
       </c>
     </row>
@@ -3496,16 +3496,16 @@
       <c r="P46" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q46" s="25">
+      <c r="Q46" s="22">
         <v>306</v>
       </c>
-      <c r="R46" s="25">
+      <c r="R46" s="22">
         <v>621</v>
       </c>
-      <c r="S46" s="25">
+      <c r="S46" s="22">
         <v>71</v>
       </c>
-      <c r="T46" s="25">
+      <c r="T46" s="22">
         <v>434</v>
       </c>
     </row>
@@ -3556,16 +3556,16 @@
       <c r="P47" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q47" s="25">
+      <c r="Q47" s="22">
         <v>99</v>
       </c>
-      <c r="R47" s="25">
+      <c r="R47" s="22">
         <v>514</v>
       </c>
-      <c r="S47" s="25">
+      <c r="S47" s="22">
         <v>92</v>
       </c>
-      <c r="T47" s="25">
+      <c r="T47" s="22">
         <v>1369</v>
       </c>
     </row>
@@ -3612,16 +3612,16 @@
       <c r="P48" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q48" s="25">
+      <c r="Q48" s="22">
         <v>196</v>
       </c>
-      <c r="R48" s="25">
+      <c r="R48" s="22">
         <v>2612</v>
       </c>
-      <c r="S48" s="25">
+      <c r="S48" s="22">
         <v>184</v>
       </c>
-      <c r="T48" s="25">
+      <c r="T48" s="22">
         <v>2276</v>
       </c>
     </row>
@@ -3666,16 +3666,16 @@
       <c r="P49" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q49" s="25">
+      <c r="Q49" s="22">
         <v>99</v>
       </c>
-      <c r="R49" s="25">
+      <c r="R49" s="22">
         <v>565</v>
       </c>
-      <c r="S49" s="25">
+      <c r="S49" s="22">
         <v>4825</v>
       </c>
-      <c r="T49" s="25">
+      <c r="T49" s="22">
         <v>10513</v>
       </c>
     </row>
@@ -3706,16 +3706,16 @@
       <c r="P50" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="Q50" s="25">
+      <c r="Q50" s="22">
         <v>6</v>
       </c>
-      <c r="R50" s="25">
+      <c r="R50" s="22">
         <v>316</v>
       </c>
-      <c r="S50" s="25">
+      <c r="S50" s="22">
         <v>25</v>
       </c>
-      <c r="T50" s="25">
+      <c r="T50" s="22">
         <v>1010</v>
       </c>
     </row>
@@ -3738,10 +3738,10 @@
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="25"/>
-      <c r="S51" s="25"/>
-      <c r="T51" s="25"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+      <c r="T51" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:A51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>